<commit_message>
Latest data: for Scottish Mon Mar 15 14:42:03 UTC 2021
</commit_message>
<xml_diff>
--- a/uk/scotland/COVID-19%2Bdaily%2Bdata%2B-%2Bby%2BNHS%2BBoard%2B-%2B15%2BMarch%2B2021.xlsx
+++ b/uk/scotland/COVID-19%2Bdaily%2Bdata%2B-%2Bby%2BNHS%2BBoard%2B-%2B15%2BMarch%2B2021.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Z617427\Objective\Director\Cache\erdm.scotland.gov.uk 8443 uA21007\A29207215\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u208525\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14030" windowHeight="11450" tabRatio="882" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14030" windowHeight="11450" tabRatio="882"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="9" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8527" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8545" uniqueCount="64">
   <si>
     <t>Date</t>
   </si>
@@ -8213,7 +8213,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -8358,11 +8358,11 @@
   </sheetPr>
   <dimension ref="A1:U394"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="64" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B343" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="84" zoomScaleNormal="64" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B364" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A376" sqref="A376"/>
+      <selection pane="bottomRight" activeCell="A378" sqref="A378"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -27244,7 +27244,54 @@
       </c>
     </row>
     <row r="377" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="B377" s="151"/>
+      <c r="A377" s="147">
+        <v>44270</v>
+      </c>
+      <c r="B377" s="122">
+        <v>15949</v>
+      </c>
+      <c r="C377" s="122">
+        <v>2847</v>
+      </c>
+      <c r="D377" s="122">
+        <v>4091</v>
+      </c>
+      <c r="E377" s="122">
+        <v>10295</v>
+      </c>
+      <c r="F377" s="122">
+        <v>11449</v>
+      </c>
+      <c r="G377" s="122">
+        <v>13846</v>
+      </c>
+      <c r="H377" s="122">
+        <v>65320</v>
+      </c>
+      <c r="I377" s="122">
+        <v>4867</v>
+      </c>
+      <c r="J377" s="122">
+        <v>38218</v>
+      </c>
+      <c r="K377" s="122">
+        <v>28937</v>
+      </c>
+      <c r="L377" s="122">
+        <v>70</v>
+      </c>
+      <c r="M377" s="122">
+        <v>214</v>
+      </c>
+      <c r="N377" s="122">
+        <v>13615</v>
+      </c>
+      <c r="O377" s="122">
+        <v>290</v>
+      </c>
+      <c r="P377" s="123">
+        <v>210008</v>
+      </c>
     </row>
     <row r="378" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B378" s="151"/>
@@ -27300,13 +27347,13 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:R188"/>
+  <dimension ref="A1:R189"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B166" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B174" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="L192" sqref="L192"/>
+      <selection pane="bottomRight" activeCell="A190" sqref="A190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -37220,6 +37267,60 @@
         <v>40</v>
       </c>
     </row>
+    <row r="189" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A189" s="36">
+        <v>44270</v>
+      </c>
+      <c r="B189" s="99" t="s">
+        <v>25</v>
+      </c>
+      <c r="C189" s="99" t="s">
+        <v>25</v>
+      </c>
+      <c r="D189" s="99" t="s">
+        <v>25</v>
+      </c>
+      <c r="E189" s="99" t="s">
+        <v>25</v>
+      </c>
+      <c r="F189" s="2">
+        <v>6</v>
+      </c>
+      <c r="G189" s="99" t="s">
+        <v>25</v>
+      </c>
+      <c r="H189" s="2">
+        <v>14</v>
+      </c>
+      <c r="I189" s="99" t="s">
+        <v>25</v>
+      </c>
+      <c r="J189" s="99" t="s">
+        <v>25</v>
+      </c>
+      <c r="K189" s="99" t="s">
+        <v>25</v>
+      </c>
+      <c r="L189" s="99" t="s">
+        <v>25</v>
+      </c>
+      <c r="M189" s="99" t="s">
+        <v>25</v>
+      </c>
+      <c r="N189" s="99" t="s">
+        <v>25</v>
+      </c>
+      <c r="O189" s="99" t="s">
+        <v>25</v>
+      </c>
+      <c r="P189" s="99" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q189" s="100">
+        <v>40</v>
+      </c>
+      <c r="R189" s="99"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:E2"/>
@@ -37235,13 +37336,13 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:R188"/>
+  <dimension ref="A1:R189"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B167" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B173" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I197" sqref="I197"/>
+      <selection pane="bottomRight" activeCell="A190" sqref="A190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -47143,6 +47244,59 @@
       </c>
       <c r="Q188" s="100">
         <v>461</v>
+      </c>
+    </row>
+    <row r="189" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A189" s="36">
+        <v>44270</v>
+      </c>
+      <c r="B189" s="2">
+        <v>42</v>
+      </c>
+      <c r="C189" s="99" t="s">
+        <v>25</v>
+      </c>
+      <c r="D189" s="2">
+        <v>7</v>
+      </c>
+      <c r="E189" s="2">
+        <v>18</v>
+      </c>
+      <c r="F189" s="2">
+        <v>45</v>
+      </c>
+      <c r="G189" s="2">
+        <v>13</v>
+      </c>
+      <c r="H189" s="2">
+        <v>152</v>
+      </c>
+      <c r="I189" s="2">
+        <v>11</v>
+      </c>
+      <c r="J189" s="2">
+        <v>55</v>
+      </c>
+      <c r="K189" s="2">
+        <v>90</v>
+      </c>
+      <c r="L189" s="99" t="s">
+        <v>25</v>
+      </c>
+      <c r="M189" s="99" t="s">
+        <v>25</v>
+      </c>
+      <c r="N189" s="2">
+        <v>7</v>
+      </c>
+      <c r="O189" s="121" t="s">
+        <v>25</v>
+      </c>
+      <c r="P189" s="121" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q189" s="100">
+        <v>447</v>
       </c>
     </row>
   </sheetData>
@@ -78697,7 +78851,7 @@
 </worksheet>
 </file>
 
-<file path=customXML/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://www.objective.com/ecm/document/metadata/53D26341A57B383EE0540010E0463CCA" version="1.0.0">
   <systemFields>
     <field name="Objective-Id">
@@ -78722,7 +78876,7 @@
       <value order="0"/>
     </field>
     <field name="Objective-ModificationStamp">
-      <value order="0">2021-03-14T11:48:41Z</value>
+      <value order="0">2021-03-15T12:35:47Z</value>
     </field>
     <field name="Objective-Owner">
       <value order="0">Grant, Neil N (u207826)</value>
@@ -78737,13 +78891,13 @@
       <value order="0">Being Drafted</value>
     </field>
     <field name="Objective-VersionId">
-      <value order="0">vA47354834</value>
+      <value order="0">vA47375334</value>
     </field>
     <field name="Objective-Version">
-      <value order="0">75.2</value>
+      <value order="0">76.1</value>
     </field>
     <field name="Objective-VersionNumber">
-      <value order="0">711</value>
+      <value order="0">714</value>
     </field>
     <field name="Objective-VersionComment">
       <value order="0"/>
@@ -78783,7 +78937,7 @@
 </metadata>
 </file>
 
-<file path=customXML/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5745109E-2DDF-40CB-AC2B-FF9B10C90820}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.objective.com/ecm/document/metadata/53D26341A57B383EE0540010E0463CCA"/>

</xml_diff>